<commit_message>
Gerbers fixed - ready to go
</commit_message>
<xml_diff>
--- a/GERBER/J0/BOM.xlsx
+++ b/GERBER/J0/BOM.xlsx
@@ -260,15 +260,13 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
BOM - Some caps cheaper at RS
</commit_message>
<xml_diff>
--- a/GERBER/J0/BOM.xlsx
+++ b/GERBER/J0/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t xml:space="preserve">J0</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">35v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECPU1C104MA5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS Australia</t>
   </si>
   <si>
     <t xml:space="preserve">47u</t>
@@ -286,19 +292,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S11" activeCellId="0" sqref="S11"/>
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.9183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,7 +325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
@@ -347,19 +352,25 @@
         <f aca="false">F3*B3*6</f>
         <v>11.286</v>
       </c>
+      <c r="J3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0.657</v>
@@ -378,13 +389,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0.048</v>
@@ -403,13 +414,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0.331</v>
@@ -428,13 +439,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0.431</v>
@@ -450,13 +461,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0.253</v>
@@ -472,16 +483,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>0.019</v>
@@ -500,10 +511,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>0.019</v>
@@ -522,10 +533,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0.019</v>
@@ -544,10 +555,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>0.019</v>
@@ -566,10 +577,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0.019</v>
@@ -588,10 +599,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>0.009</v>
@@ -617,7 +628,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>2</v>
@@ -637,13 +648,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>0.431</v>
@@ -657,7 +668,7 @@
         <v>5.172</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
         <v>1</v>
       </c>
@@ -681,19 +692,25 @@
         <f aca="false">F18*12</f>
         <v>7.524</v>
       </c>
+      <c r="J18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>0.657</v>
@@ -712,10 +729,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>0.978</v>
@@ -734,10 +751,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1.89</v>
@@ -753,16 +770,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>0.012</v>
@@ -778,16 +795,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>2.55</v>
@@ -813,7 +830,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>2</v>
@@ -827,13 +844,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0.616</v>
@@ -849,13 +866,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>1.49</v>
@@ -871,13 +888,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>4.69</v>
@@ -892,13 +909,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>2.1</v>
@@ -912,13 +929,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>0.118</v>

</xml_diff>